<commit_message>
Capture | 2024.10.14(MON) 02:54
- todo.txt 파일 참고
</commit_message>
<xml_diff>
--- a/preprocessing/directory_mapping.xlsx
+++ b/preprocessing/directory_mapping.xlsx
@@ -448,840 +448,840 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>가치</t>
+          <t>│¬└╠</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>0001</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>감사</t>
+          <t>│¬┤⌐┤┘</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>0002</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>걱정</t>
+          <t>│¬┼╕│¬┤┘</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>0003</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>건강</t>
+          <t>│¬░í┤┘</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>0004</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>결정</t>
+          <t>│δ╖┬</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>0005</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>경험</t>
+          <t>│ε┤┘</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>0006</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>계획</t>
+          <t>│ε╢≤┤┘</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>0007</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>고민</t>
+          <t>│⌡─í┤┘</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>0008</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>고통</t>
+          <t>│╖┤┘</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>8</t>
+          <t>0009</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>공부</t>
+          <t>│╗└╧</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>0010</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>관심</t>
+          <t>│╗╕«┤┘</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>0011</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>교육</t>
+          <t>│╗╖┴│⌡┤┘</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>11</t>
+          <t>0012</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>기대</t>
+          <t>│╤┤┘</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>12</t>
+          <t>0013</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>기분</t>
+          <t>│╤╛ε┐└┤┘</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>13</t>
+          <t>0014</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>기쁨</t>
+          <t>│╩</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>14</t>
+          <t>0015</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>기억</t>
+          <t>│▓└┌</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>15</t>
+          <t>0016</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>기적</t>
+          <t>│▓┤┘</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>16</t>
+          <t>0017</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>기회</t>
+          <t>│▓▒Γ┤┘</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>17</t>
+          <t>0018</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>나가다</t>
+          <t>┐°╟╧┤┘</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>18</t>
+          <t>0019</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>나누다</t>
+          <t>┐⌠┤┘</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>19</t>
+          <t>0020</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>나이</t>
+          <t>┐└┤├</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>0021</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>나타나다</t>
+          <t>┐┬╡╡</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>21</t>
+          <t>0022</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>남기다</t>
+          <t>┐╓</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>0023</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>남다</t>
+          <t>└╘┐°</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>0024</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>남자</t>
+          <t>└╠╕º</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>24</t>
+          <t>0025</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>낮다</t>
+          <t>└╠╟╪</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>25</t>
+          <t>0026</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>내려놓다</t>
+          <t>└╥╛ε╣÷╕«┤┘</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>26</t>
+          <t>0027</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>내리다</t>
+          <t>└╧║╬╖»</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>27</t>
+          <t>0028</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>내일</t>
+          <t>└╪┤┘</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>28</t>
+          <t>0029</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>너</t>
+          <t>┤÷║╨┐í</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>29</t>
+          <t>0030</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>넘다</t>
+          <t>┤δ╚¡</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>30</t>
+          <t>0031</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>넘어오다</t>
+          <t>┤⌐▒╕</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>31</t>
+          <t>0032</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>노력</t>
+          <t>┤┘└╜</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>32</t>
+          <t>0033</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>놀다</t>
+          <t>┤┘╕«</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>33</t>
+          <t>0034</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>놀라다</t>
+          <t>┤├╛ε│¬┤┘</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>34</t>
+          <t>0035</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>놓치다</t>
+          <t>┤▌┤┘</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>0036</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>누구</t>
+          <t>╛α╝╙</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>36</t>
+          <t>0037</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>늘어나다</t>
+          <t>╛ε┴÷╖┤┤┘</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>37</t>
+          <t>0038</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>다리</t>
+          <t>╛ε╕░└╠</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>38</t>
+          <t>0039</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>다음</t>
+          <t>╛ε╖╞┤┘</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>39</t>
+          <t>0040</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>닫다</t>
+          <t>╛ε╢╗░╘</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>0041</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>대화</t>
+          <t>╛╚│τ╟╧╝╝┐Σ</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>41</t>
+          <t>0042</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>덕분에</t>
+          <t>╛╚┼╕▒⌡┤┘</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>42</t>
+          <t>0043</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>도움</t>
+          <t>╛╚╜╔</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>43</t>
+          <t>0044</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>독서</t>
+          <t>╛╞│ó┤┘</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>44</t>
+          <t>0045</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>아끼다</t>
+          <t>╛╞╕º┤Σ┤┘</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>45</t>
+          <t>0046</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>아름답다</t>
+          <t>╛╦┤┘</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>46</t>
+          <t>0047</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>안녕하세요</t>
+          <t>╛╦╖┴┴╓┤┘</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>47</t>
+          <t>0048</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>안심</t>
+          <t>╛╦╛╞┬≈╕«┤┘</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>48</t>
+          <t>0049</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>안타깝다</t>
+          <t>╛╦╛╞╝¡╟╧┤┘</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>49</t>
+          <t>0050</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>알다</t>
+          <t>╡╡┐≥</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>50</t>
+          <t>0051</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>알려주다</t>
+          <t>╡╢╝¡</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>51</t>
+          <t>0052</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>알아서하다</t>
+          <t>░°║╬</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>0053</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>알아차리다</t>
+          <t>░µ╟Φ</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>53</t>
+          <t>0054</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>약속</t>
+          <t>░¿╗τ</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>54</t>
+          <t>0055</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>어떻게</t>
+          <t>░í─í</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>55</t>
+          <t>0056</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>어렵다</t>
+          <t>░ß┴ñ</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>56</t>
+          <t>0057</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>어린이</t>
+          <t>░φ┼δ</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>57</t>
+          <t>0058</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>어지럽다</t>
+          <t>░Φ╚╣</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>58</t>
+          <t>0059</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>오늘</t>
+          <t>░φ╣╬</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>59</t>
+          <t>0060</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>온도</t>
+          <t>░ⁿ╜╔</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>60</t>
+          <t>0061</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>왜</t>
+          <t>░╞┴ñ</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>61</t>
+          <t>0062</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>웃다</t>
+          <t>░╟░¡</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>0063</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>원하다</t>
+          <t>▒Γ└√</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>63</t>
+          <t>0064</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>이름</t>
+          <t>▒Γ┤δ</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>64</t>
+          <t>0065</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>이해</t>
+          <t>▒Γ║╨</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>65</t>
+          <t>0066</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>일부러</t>
+          <t>▒Γ╗▌</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>66</t>
+          <t>0067</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>잃어버리다</t>
+          <t>▒Γ╚╕</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>67</t>
+          <t>0068</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>입원</t>
+          <t>▒Γ╛∩</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>68</t>
+          <t>0069</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>잊다</t>
+          <t>▒│└░</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>69</t>
+          <t>0070</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Capture | 2024.10.14(MON) 21:32
</commit_message>
<xml_diff>
--- a/preprocessing/directory_mapping.xlsx
+++ b/preprocessing/directory_mapping.xlsx
@@ -448,7 +448,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>│¬└╠</t>
+          <t>가치</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -460,7 +460,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>│¬┤⌐┤┘</t>
+          <t>감사</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -472,7 +472,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>│¬┼╕│¬┤┘</t>
+          <t>걱정</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -484,7 +484,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>│¬░í┤┘</t>
+          <t>건강</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -496,7 +496,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>│δ╖┬</t>
+          <t>결정</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -508,7 +508,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>│ε┤┘</t>
+          <t>경험</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -520,7 +520,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>│ε╢≤┤┘</t>
+          <t>계획</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -532,7 +532,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>│⌡─í┤┘</t>
+          <t>고민</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -544,7 +544,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>│╖┤┘</t>
+          <t>고통</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -556,7 +556,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>│╗└╧</t>
+          <t>공부</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -568,7 +568,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>│╗╕«┤┘</t>
+          <t>관심</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -580,7 +580,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>│╗╖┴│⌡┤┘</t>
+          <t>교육</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -592,7 +592,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>│╤┤┘</t>
+          <t>기대</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -604,7 +604,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>│╤╛ε┐└┤┘</t>
+          <t>기분</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -616,7 +616,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>│╩</t>
+          <t>기쁨</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -628,7 +628,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>│▓└┌</t>
+          <t>기억</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -640,7 +640,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>│▓┤┘</t>
+          <t>기적</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -652,7 +652,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>│▓▒Γ┤┘</t>
+          <t>기회</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -664,7 +664,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>┐°╟╧┤┘</t>
+          <t>나가다</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -676,7 +676,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>┐⌠┤┘</t>
+          <t>나누다</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -688,7 +688,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>┐└┤├</t>
+          <t>나이</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -700,7 +700,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>┐┬╡╡</t>
+          <t>나타나다</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -712,7 +712,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>┐╓</t>
+          <t>남기다</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -724,7 +724,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>└╘┐°</t>
+          <t>남다</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -736,7 +736,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>└╠╕º</t>
+          <t>남자</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -748,7 +748,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>└╠╟╪</t>
+          <t>낮다</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -760,7 +760,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>└╥╛ε╣÷╕«┤┘</t>
+          <t>내려놓다</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -772,7 +772,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>└╧║╬╖»</t>
+          <t>내리다</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -784,7 +784,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>└╪┤┘</t>
+          <t>내일</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -796,7 +796,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>┤÷║╨┐í</t>
+          <t>너</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -808,7 +808,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>┤δ╚¡</t>
+          <t>넘다</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -820,7 +820,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>┤⌐▒╕</t>
+          <t>넘어오다</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -832,7 +832,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>┤┘└╜</t>
+          <t>노력</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -844,7 +844,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>┤┘╕«</t>
+          <t>놀다</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -856,7 +856,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>┤├╛ε│¬┤┘</t>
+          <t>놀라다</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -868,7 +868,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>┤▌┤┘</t>
+          <t>놓치다</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -880,7 +880,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>╛α╝╙</t>
+          <t>누구</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -892,7 +892,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>╛ε┴÷╖┤┤┘</t>
+          <t>늘어나다</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -904,7 +904,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>╛ε╕░└╠</t>
+          <t>다리</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -916,7 +916,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>╛ε╖╞┤┘</t>
+          <t>다음</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -928,7 +928,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>╛ε╢╗░╘</t>
+          <t>닫다</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -940,7 +940,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>╛╚│τ╟╧╝╝┐Σ</t>
+          <t>대화</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -952,7 +952,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>╛╚┼╕▒⌡┤┘</t>
+          <t>덕분에</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -964,7 +964,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>╛╚╜╔</t>
+          <t>도움</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -976,7 +976,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>╛╞│ó┤┘</t>
+          <t>독서</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -988,7 +988,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>╛╞╕º┤Σ┤┘</t>
+          <t>아끼다</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1000,7 +1000,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>╛╦┤┘</t>
+          <t>아름답다</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1012,7 +1012,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>╛╦╖┴┴╓┤┘</t>
+          <t>안녕하세요</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1024,7 +1024,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>╛╦╛╞┬≈╕«┤┘</t>
+          <t>안심</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1036,7 +1036,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>╛╦╛╞╝¡╟╧┤┘</t>
+          <t>안타깝다</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1048,7 +1048,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>╡╡┐≥</t>
+          <t>알다</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1060,7 +1060,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>╡╢╝¡</t>
+          <t>알리다(알려주다)</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1072,7 +1072,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>░°║╬</t>
+          <t>알아서하다</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1084,7 +1084,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>░µ╟Φ</t>
+          <t>알아차리다</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1096,7 +1096,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>░¿╗τ</t>
+          <t>약속</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1108,7 +1108,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>░í─í</t>
+          <t>어떻게</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1120,7 +1120,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>░ß┴ñ</t>
+          <t>어렵다</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1132,7 +1132,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>░φ┼δ</t>
+          <t>어린이</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1144,7 +1144,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>░Φ╚╣</t>
+          <t>어지럽다</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1156,7 +1156,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>░φ╣╬</t>
+          <t>오늘</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1168,7 +1168,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>░ⁿ╜╔</t>
+          <t>온도</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -1180,7 +1180,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>░╞┴ñ</t>
+          <t>왜</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -1192,7 +1192,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>░╟░¡</t>
+          <t>웃다</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1204,7 +1204,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>▒Γ└√</t>
+          <t>원하다</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1216,7 +1216,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>▒Γ┤δ</t>
+          <t>이름</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1228,7 +1228,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>▒Γ║╨</t>
+          <t>이해</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -1240,7 +1240,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>▒Γ╗▌</t>
+          <t>일부러</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -1252,7 +1252,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>▒Γ╚╕</t>
+          <t>잃어버리다</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -1264,7 +1264,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>▒Γ╛∩</t>
+          <t>입원</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -1276,7 +1276,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>▒│└░</t>
+          <t>잊다</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">

</xml_diff>